<commit_message>
Tables of XS including 1.8
</commit_message>
<xml_diff>
--- a/01_signal_production/Data_Generation_woRHC/Data_5K_13_TeV/lq_lq/Cross_Sections/XS_Matriz.xlsx
+++ b/01_signal_production/Data_Generation_woRHC/Data_5K_13_TeV/lq_lq/Cross_Sections/XS_Matriz.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,50 +436,35 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>1750</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>1250</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>2250</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>1750</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>2250</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -492,33 +477,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>932.7</v>
+        <v>0.1974</v>
       </c>
       <c r="C2" t="n">
-        <v>19.85</v>
+        <v>0.0333</v>
       </c>
       <c r="D2" t="n">
-        <v>1.523</v>
+        <v>0.006502</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1974</v>
+        <v>0.001415</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0333</v>
+        <v>0.0003296</v>
       </c>
       <c r="G2" t="n">
-        <v>0.006502</v>
+        <v>7.954e-05</v>
       </c>
       <c r="H2" t="n">
-        <v>0.001415</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.0003296</v>
-      </c>
-      <c r="J2" t="n">
-        <v>7.954e-05</v>
-      </c>
-      <c r="K2" t="n">
         <v>1.98e-05</v>
       </c>
     </row>
@@ -529,33 +505,24 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>929.1</v>
+        <v>0.196</v>
       </c>
       <c r="C3" t="n">
-        <v>19.93</v>
+        <v>0.03336</v>
       </c>
       <c r="D3" t="n">
-        <v>1.518</v>
+        <v>0.006538</v>
       </c>
       <c r="E3" t="n">
-        <v>0.196</v>
+        <v>0.001414</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03336</v>
+        <v>0.0003285</v>
       </c>
       <c r="G3" t="n">
-        <v>0.006538</v>
+        <v>7.96e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001414</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.0003285</v>
-      </c>
-      <c r="J3" t="n">
-        <v>7.96e-05</v>
-      </c>
-      <c r="K3" t="n">
         <v>1.986e-05</v>
       </c>
     </row>
@@ -566,33 +533,24 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>925.5</v>
+        <v>0.1971</v>
       </c>
       <c r="C4" t="n">
-        <v>19.99</v>
+        <v>0.03331</v>
       </c>
       <c r="D4" t="n">
-        <v>1.533</v>
+        <v>0.006535</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1971</v>
+        <v>0.001416</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03331</v>
+        <v>0.0003302</v>
       </c>
       <c r="G4" t="n">
-        <v>0.006535</v>
+        <v>7.931e-05</v>
       </c>
       <c r="H4" t="n">
-        <v>0.001416</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.0003302</v>
-      </c>
-      <c r="J4" t="n">
-        <v>7.931e-05</v>
-      </c>
-      <c r="K4" t="n">
         <v>1.981e-05</v>
       </c>
     </row>
@@ -603,181 +561,164 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>932.3</v>
+        <v>0.1969</v>
       </c>
       <c r="C5" t="n">
-        <v>20</v>
+        <v>0.03326</v>
       </c>
       <c r="D5" t="n">
-        <v>1.528</v>
+        <v>0.006532</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1969</v>
+        <v>0.001418</v>
       </c>
       <c r="F5" t="n">
-        <v>0.03326</v>
+        <v>0.0003282</v>
       </c>
       <c r="G5" t="n">
-        <v>0.006532</v>
+        <v>7.983999999999999e-05</v>
       </c>
       <c r="H5" t="n">
-        <v>0.001418</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.0003282</v>
-      </c>
-      <c r="J5" t="n">
-        <v>7.983999999999999e-05</v>
-      </c>
-      <c r="K5" t="n">
         <v>1.987e-05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>940.8</v>
+        <v>0.1982092</v>
       </c>
       <c r="C6" t="n">
-        <v>20.15</v>
+        <v>0.03347837</v>
       </c>
       <c r="D6" t="n">
-        <v>1.539</v>
+        <v>0.006548228</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1988</v>
+        <v>0.0014225013</v>
       </c>
       <c r="F6" t="n">
-        <v>0.03358</v>
+        <v>0.00033068328</v>
       </c>
       <c r="G6" t="n">
-        <v>0.006568</v>
+        <v>7.9878115e-05</v>
       </c>
       <c r="H6" t="n">
-        <v>0.001436</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.0003313</v>
-      </c>
-      <c r="J6" t="n">
-        <v>7.972e-05</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1.999e-05</v>
+        <v>1.9879499e-05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>952.6</v>
+        <v>0.1988</v>
       </c>
       <c r="C7" t="n">
-        <v>20.49</v>
+        <v>0.03358</v>
       </c>
       <c r="D7" t="n">
-        <v>1.567</v>
+        <v>0.006568</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2026</v>
+        <v>0.001436</v>
       </c>
       <c r="F7" t="n">
-        <v>0.03419</v>
+        <v>0.0003313</v>
       </c>
       <c r="G7" t="n">
-        <v>0.006678</v>
+        <v>7.972e-05</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00145</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.0003353</v>
-      </c>
-      <c r="J7" t="n">
-        <v>8.069e-05</v>
-      </c>
-      <c r="K7" t="n">
-        <v>2.009e-05</v>
+        <v>1.999e-05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>981.8</v>
+        <v>0.2026</v>
       </c>
       <c r="C8" t="n">
-        <v>21.14</v>
+        <v>0.03419</v>
       </c>
       <c r="D8" t="n">
-        <v>1.616</v>
+        <v>0.006678</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2086</v>
+        <v>0.00145</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03522</v>
+        <v>0.0003353</v>
       </c>
       <c r="G8" t="n">
-        <v>0.006843</v>
+        <v>8.069e-05</v>
       </c>
       <c r="H8" t="n">
-        <v>0.001482</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.0003419</v>
-      </c>
-      <c r="J8" t="n">
-        <v>8.231e-05</v>
-      </c>
-      <c r="K8" t="n">
-        <v>2.033e-05</v>
+        <v>2.009e-05</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.2086</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.03522</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.006843</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.001482</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0003419</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8.231e-05</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2.033e-05</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>3.5</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>1021</v>
-      </c>
-      <c r="C9" t="n">
-        <v>22.2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.714</v>
-      </c>
-      <c r="E9" t="n">
+      <c r="B10" t="n">
         <v>0.219</v>
       </c>
-      <c r="F9" t="n">
+      <c r="C10" t="n">
         <v>0.03666</v>
       </c>
-      <c r="G9" t="n">
+      <c r="D10" t="n">
         <v>0.00716</v>
       </c>
-      <c r="H9" t="n">
+      <c r="E10" t="n">
         <v>0.001549</v>
       </c>
-      <c r="I9" t="n">
+      <c r="F10" t="n">
         <v>0.0003576</v>
       </c>
-      <c r="J9" t="n">
+      <c r="G10" t="n">
         <v>8.500000000000001e-05</v>
       </c>
-      <c r="K9" t="n">
+      <c r="H10" t="n">
         <v>2.092e-05</v>
       </c>
     </row>

</xml_diff>